<commit_message>
working on currating the data
</commit_message>
<xml_diff>
--- a/data/LMini_iNat_Pops_filtered_metadata.xlsx
+++ b/data/LMini_iNat_Pops_filtered_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\Documents\R\Lepto_iNat_Pops\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\Documents\R\Data_Sci_Leptosiphon_Polymorphism\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54780790-58D9-4A99-B77D-8B8789AC6B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E99A2A2-C504-4F4A-820F-AF11DACEBF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="0" windowWidth="9276" windowHeight="12336" xr2:uid="{2DDA18C5-069F-4AEC-9FB6-1E496F22AE95}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2DDA18C5-069F-4AEC-9FB6-1E496F22AE95}"/>
   </bookViews>
   <sheets>
     <sheet name="LMini_iNat_Pops_filtered" sheetId="1" r:id="rId1"/>
@@ -1077,13 +1077,14 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I35"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="4" customWidth="1"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1162,7 +1163,7 @@
         <v>-122.6432183333</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f t="shared" ref="E3:E35" si="0">HYPERLINK(B3)</f>
+        <f t="shared" ref="E3:E34" si="0">HYPERLINK(B3)</f>
         <v>https://www.inaturalist.org/observations/27733914</v>
       </c>
       <c r="F3">

</xml_diff>